<commit_message>
some changes to Day1 file
</commit_message>
<xml_diff>
--- a/docs/modules/computer-statistics/Day1.xlsx
+++ b/docs/modules/computer-statistics/Day1.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Event Numbers" sheetId="3" r:id="rId3"/>
+    <sheet name="Odd" sheetId="4" r:id="rId4"/>
+    <sheet name="Dice Roll Samples" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>A simple random sample is a subset of  a statistical population in which each member of the subset has an equal probability of being chosen.</t>
   </si>
@@ -35,6 +37,9 @@
   </si>
   <si>
     <t>Even #</t>
+  </si>
+  <si>
+    <t>Odd #</t>
   </si>
 </sst>
 </file>
@@ -365,92 +370,92 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>10</v>
+        <f t="shared" ref="A2:A16" ca="1" si="0">RANDBETWEEN(1,175)</f>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>27</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>35</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>44</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>53</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>57</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>66</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>74</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>78</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>89</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>124</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>141</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>153</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>154</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f ca="1">RANDBETWEEN(1,175)</f>
-        <v>164</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -485,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
@@ -1037,4 +1042,1742 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B251"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>37</v>
+      </c>
+      <c r="B20">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>49</v>
+      </c>
+      <c r="B26">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>59</v>
+      </c>
+      <c r="B31">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>61</v>
+      </c>
+      <c r="B32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>63</v>
+      </c>
+      <c r="B33">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>65</v>
+      </c>
+      <c r="B34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>67</v>
+      </c>
+      <c r="B35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>69</v>
+      </c>
+      <c r="B36">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>71</v>
+      </c>
+      <c r="B37">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>73</v>
+      </c>
+      <c r="B38">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>75</v>
+      </c>
+      <c r="B39">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>77</v>
+      </c>
+      <c r="B40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>79</v>
+      </c>
+      <c r="B41">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>81</v>
+      </c>
+      <c r="B42">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>83</v>
+      </c>
+      <c r="B43">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>85</v>
+      </c>
+      <c r="B44">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>87</v>
+      </c>
+      <c r="B45">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>89</v>
+      </c>
+      <c r="B46">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>91</v>
+      </c>
+      <c r="B47">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>93</v>
+      </c>
+      <c r="B48">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>95</v>
+      </c>
+      <c r="B49">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>97</v>
+      </c>
+      <c r="B50">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>99</v>
+      </c>
+      <c r="B51">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>499</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f ca="1">RANDBETWEEN(1,6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f t="shared" ref="A2:A50" ca="1" si="0">RANDBETWEEN(1,6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>